<commit_message>
comments added, Read me file has been added and log book has been updated.
</commit_message>
<xml_diff>
--- a/LogBook.xlsx
+++ b/LogBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\5011 CEM My submission files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCC5E4A-D8D9-48C0-A609-1F7BB3180FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A80AD8-B208-44DF-8004-3E388E1B4F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="0" windowWidth="13100" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Start Date</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>There was a lot of trial and error in writing all of these tasks and it has shown me how much important project planning can be. I have leraned that moving from programing langues can be a bit easier then I initially thought and I have changed my apporoach to that. In the begening i was struggling with the basic maths work but i had no understanding of what the code was actually doing after learing about the help function i was able to do all the task without much effort. I could have made my error testing code a bit better by using the same script for -9999 and NaN  error automation and generation codes. I will try to take this experince and focus more on the planing side of pograming from now on as i could have done most of this programming optimally if i had just done that from the start.</t>
+  </si>
+  <si>
+    <t>I need to improve my report for final submission. I need to add tables. I need to review the code and make changes if needed.</t>
+  </si>
+  <si>
+    <t>Tables have been added to the report.  Comments have been added to the code to help the user understand the code better.</t>
   </si>
 </sst>
 </file>
@@ -465,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +712,7 @@
         <v>44243</v>
       </c>
       <c r="B15" s="2">
-        <v>44316</v>
+        <v>44313</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>33</v>
@@ -718,9 +724,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>44314</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44314</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="3"/>

</xml_diff>

<commit_message>
spelling mistakes corrected and tables formatted
</commit_message>
<xml_diff>
--- a/LogBook.xlsx
+++ b/LogBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\5011CEM_Saad_Iftikhar_9789180\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\5011 CEM\5011CEM Git Clone\5011CEM\5011CEM2021iftikhars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB679F-511A-4E69-B926-CBFA0001BBC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9212A0-AB7C-4D9E-A753-CC23D2EA9FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Achieved work</t>
   </si>
   <si>
-    <t>I started making gantt charts.</t>
-  </si>
-  <si>
     <t>Now I need to do the task for the parallel processing week.</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>I got some feedback from Richard he said my video had all the content but was lacking speed.</t>
   </si>
   <si>
-    <t>I need to finsh the viva video.</t>
-  </si>
-  <si>
     <t>I have made the viva video.</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>I still haven't been able to do the tasks for week 2 properly I need to ask Richard to help me understand them better or learn basic MATLAB.</t>
   </si>
   <si>
-    <t xml:space="preserve">I have asked richard what to do he has helped me, and I can write functions I MATLAB. </t>
-  </si>
-  <si>
     <t>Scripts work like python separate pages and functions in both languages act the same, but the syntax is different.</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
     <t>I have done initial automation testing.</t>
   </si>
   <si>
-    <t>I don't think I understand completely what automation is or how it would be defined by other people. I don't know if I'll have to automate the whole test or just the error tests. I need to ask Richard and some of my friends as they would know better. I wasn’t able to attend the lecture but my friends asked Richard about Amdahl’s law so i need to ask them about that later.</t>
-  </si>
-  <si>
     <t>I have made a basic husk for the overall project. I can use this to build the full-scale project later. I have manged to automate the graphs and the error tests.</t>
   </si>
   <si>
@@ -143,16 +131,28 @@
     <t xml:space="preserve">I still managed to do a lot of work. As the essemblevectorpar was still giving me a issue I manged to solve the problem by adding the code under the for loop so it doesn’t change size as often and I did the same for T3 as my time was coming inaccurate. I have also made a initial video for the viva so if the worst case happens i can at least pass the Viva. The content of the video is good, but the audio quality is quite bad. </t>
   </si>
   <si>
-    <t>I have ordered a head set to improve my audio quality but it doesn’t work. I have called the Microsoft Team and installed all the software but still my audio quality is quite bad. I have downloaded some audio software to improve the audio quality, but they don't work either. I've found an app called Krisp which has improved the audio quality. Now i can solely focus on 5011 related work and finish my project.</t>
-  </si>
-  <si>
     <t>I need to learn MATLAB properly. I need to improve my flow charts. I need to automate everything. I need to write my report.</t>
   </si>
   <si>
     <t>I didn't learn MATLAB but one of my friends has told me about MATLABS help function which has made doing all the tasks trivial. I have improved my flow charts. I have automated everything, but I am using interp1 to give recommended processors after researching i have concluded that polyfit works better for this i have decided to use it. Everything works as intended. I have written my report.</t>
   </si>
   <si>
-    <t>There was a lot of trial and error in writing all these tasks and it has shown me how much important project planning can be. I have learned that moving from programming languages can be a bit easier than I initially thought and I have changed my approach to that. In the beginning i was struggling with the basic maths work but i had no understanding of what the code was actually doing after learning about the help function i was able to do all the task without much effort. I could have made my error testing code a bit better by using the same script for -9999 and NaN  error automation and generation codes. I will try to take this experience and focus more on the planning side of programming from now on as i could have done most of this programming optimally if i had just done that from the start.</t>
+    <t>I started making Gantt charts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have asked Richard what to do he has helped me, and I can write functions I MATLAB. </t>
+  </si>
+  <si>
+    <t>I need to finish the viva video.</t>
+  </si>
+  <si>
+    <t>I don't think I understand completely what automation is or how it would be defined by other people. I don't know if I'll have to automate the whole test or just the error tests. I need to ask Richard and some of my friends as they would know better. I couldn’t attend the lecture, but my friends asked Richard about Amdahl’s law, so I need to ask them about that later.</t>
+  </si>
+  <si>
+    <t>I have ordered a head set to improve my audio quality, but it doesn’t work. I have called the Microsoft Team and installed all the software but still my audio quality is quite bad. I have downloaded some audio software to improve the audio quality, but they don't work either. I've found an app called Krisp which has improved the audio quality. Now i can solely focus on 5011 related work and finish my project.</t>
+  </si>
+  <si>
+    <t>There was a lot of trial and error in writing all these tasks and it has shown me how much important project planning can be. I have learned that moving from programming languages can be a bit easier than I initially thought and I have changed my approach to that. In the beginning i was struggling with the basic maths work but I had no understanding of what the code was doing after learning about the help function, I was able to do all the task without much effort. I could have made my error testing code a bit better by using the same script for -9999 and NaN  error automation and generation codes. I will try to take this experience and focus more on the planning side of programming from now on as i could have done most of this programming optimally if I had just done that from the start.</t>
   </si>
 </sst>
 </file>
@@ -183,15 +183,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,34 +205,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,327 +599,329 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="5" width="50.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="50.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4">
+        <v>44217</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44217</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F2" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9">
+        <v>44224</v>
+      </c>
+      <c r="B3" s="10">
+        <v>44224</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4">
+        <v>44231</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44231</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>44217</v>
-      </c>
-      <c r="B2" s="6">
-        <v>44217</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9">
+        <v>44238</v>
+      </c>
+      <c r="B5" s="10">
+        <v>44238</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4">
+        <v>44238</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44243</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F6" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9">
+        <v>44245</v>
+      </c>
+      <c r="B7" s="10">
+        <v>44245</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4">
+        <v>44252</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44252</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9">
+        <v>44259</v>
+      </c>
+      <c r="B9" s="10">
+        <v>44259</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>44224</v>
-      </c>
-      <c r="B3" s="6">
-        <v>44224</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>44231</v>
-      </c>
-      <c r="B4" s="6">
-        <v>44231</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>44238</v>
-      </c>
-      <c r="B5" s="6">
-        <v>44238</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>44238</v>
-      </c>
-      <c r="B6" s="6">
+    <row r="10" spans="1:6" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4">
+        <v>44260</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44271</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9">
+        <v>44272</v>
+      </c>
+      <c r="B11" s="10">
+        <v>44274</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4">
+        <v>44275</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44279</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9">
+        <v>44280</v>
+      </c>
+      <c r="B13" s="10">
+        <v>44300</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4">
+        <v>44300</v>
+      </c>
+      <c r="B14" s="5">
         <v>44243</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="C14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="218" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>44243</v>
+      </c>
+      <c r="B15" s="10">
+        <v>44313</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>44245</v>
-      </c>
-      <c r="B7" s="6">
-        <v>44245</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>44252</v>
-      </c>
-      <c r="B8" s="6">
-        <v>44252</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>44259</v>
-      </c>
-      <c r="B9" s="6">
-        <v>44259</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>44260</v>
-      </c>
-      <c r="B10" s="6">
-        <v>44271</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="5">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>44272</v>
-      </c>
-      <c r="B11" s="6">
-        <v>44274</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="D15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="4">
+        <v>44314</v>
+      </c>
+      <c r="B16" s="5">
+        <v>44314</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>44275</v>
-      </c>
-      <c r="B12" s="6">
-        <v>44279</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="5">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>44280</v>
-      </c>
-      <c r="B13" s="6">
-        <v>44300</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>44300</v>
-      </c>
-      <c r="B14" s="6">
-        <v>44243</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="D16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
-        <v>44243</v>
-      </c>
-      <c r="B15" s="6">
-        <v>44313</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>44314</v>
-      </c>
-      <c r="B16" s="6">
-        <v>44314</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>